<commit_message>
added extent repoting and data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/simple.xlsx
+++ b/src/test/resources/testData/simple.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="tc_01" sheetId="1" r:id="rId1"/>
-    <sheet name="tc_02" sheetId="3" r:id="rId2"/>
-    <sheet name="tc_03" sheetId="4" r:id="rId3"/>
-    <sheet name="tc_04" sheetId="5" r:id="rId4"/>
-    <sheet name="tc_05" sheetId="6" r:id="rId5"/>
-    <sheet name="tc_06" sheetId="7" r:id="rId6"/>
-    <sheet name="testData" sheetId="8" r:id="rId7"/>
+    <sheet name="tc_02" sheetId="3" r:id="rId1"/>
+    <sheet name="tc_03" sheetId="4" r:id="rId2"/>
+    <sheet name="tc_04" sheetId="5" r:id="rId3"/>
+    <sheet name="tc_05" sheetId="6" r:id="rId4"/>
+    <sheet name="tc_06" sheetId="7" r:id="rId5"/>
+    <sheet name="testData" sheetId="8" r:id="rId6"/>
+    <sheet name="validateFBLoginWIthValidCred" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -52,9 +52,6 @@
     <t>tc_02</t>
   </si>
   <si>
-    <t>tc_01</t>
-  </si>
-  <si>
     <t>esdf</t>
   </si>
   <si>
@@ -73,22 +70,28 @@
     <t>dsdfsdf</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastaname</t>
-  </si>
-  <si>
-    <t>verifyLoginWithValidCred</t>
-  </si>
-  <si>
     <t>w2ajava@way2automation.com</t>
   </si>
   <si>
     <t>Tcs@12345</t>
+  </si>
+  <si>
+    <t>rahul.jhajava@kljflkjds</t>
+  </si>
+  <si>
+    <t>kjkasldj</t>
+  </si>
+  <si>
+    <t>sdsdf</t>
+  </si>
+  <si>
+    <t>asdsad</t>
+  </si>
+  <si>
+    <t>validateFBLoginWIthValidCred</t>
+  </si>
+  <si>
+    <t>tc_03</t>
   </si>
 </sst>
 </file>
@@ -135,9 +138,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,28 +449,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>8744954505</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>12345</v>
+        <v>4545645</v>
       </c>
     </row>
   </sheetData>
@@ -478,25 +480,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>12345</v>
+        <v>56767567</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +526,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>12345</v>
@@ -555,7 +557,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>12345</v>
@@ -567,37 +569,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -628,12 +599,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -641,12 +612,12 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -654,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>8744954505</v>
       </c>
@@ -662,58 +633,49 @@
         <v>12123</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -721,12 +683,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -735,4 +697,51 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>